<commit_message>
Median time, Q1, Q3 corrected
</commit_message>
<xml_diff>
--- a/Results/Results table.xlsx
+++ b/Results/Results table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14340" windowHeight="4215" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14340" windowHeight="4215"/>
   </bookViews>
   <sheets>
     <sheet name="FU time" sheetId="5" r:id="rId1"/>
@@ -74,21 +74,6 @@
     <t>n</t>
   </si>
   <si>
-    <t>4.79 [4.60; 4.94]</t>
-  </si>
-  <si>
-    <t>4.75 [4.48; 4.98]</t>
-  </si>
-  <si>
-    <t>2.73 [2.46; 3.03]</t>
-  </si>
-  <si>
-    <t>6.33 [6.06; 7.07]</t>
-  </si>
-  <si>
-    <t>6.19 [5.91; 6.73]</t>
-  </si>
-  <si>
     <t>[0.75; 0.78]</t>
   </si>
   <si>
@@ -431,9 +416,6 @@
     <t>[2.65; 19.94]</t>
   </si>
   <si>
-    <t>5.02 [4.89; 5.14]</t>
-  </si>
-  <si>
     <t>Validation</t>
   </si>
   <si>
@@ -485,24 +467,6 @@
     <t>n.MSM</t>
   </si>
   <si>
-    <t>4.87 [4.67; 5.01]</t>
-  </si>
-  <si>
-    <t>4.82 [4.52; 5.06]</t>
-  </si>
-  <si>
-    <t>2.69 [2.46; 2.99]</t>
-  </si>
-  <si>
-    <t>6.47 [6.09; 7.20]</t>
-  </si>
-  <si>
-    <t>6.49 [6.07; 6.93]</t>
-  </si>
-  <si>
-    <t>4.84 [4.70; 4.99]</t>
-  </si>
-  <si>
     <t>Recurrence time</t>
   </si>
   <si>
@@ -531,6 +495,42 @@
   </si>
   <si>
     <t>e2</t>
+  </si>
+  <si>
+    <t>4.87 [2.29; 7.77]</t>
+  </si>
+  <si>
+    <t>4.82 [2.99; 6.94]</t>
+  </si>
+  <si>
+    <t>2.69 [0.93; 5.52]</t>
+  </si>
+  <si>
+    <t>6.47 [3.65; 9.65]</t>
+  </si>
+  <si>
+    <t>6.49 [3.62; 10.19]</t>
+  </si>
+  <si>
+    <t>4.84 [2.16; 8.67]</t>
+  </si>
+  <si>
+    <t>4.79 [2.28; 7.76]</t>
+  </si>
+  <si>
+    <t>4.75 [2.97; 6.96]</t>
+  </si>
+  <si>
+    <t>2.73 [0.94; 5.56]</t>
+  </si>
+  <si>
+    <t>6.33 [3.53; 9.60]</t>
+  </si>
+  <si>
+    <t>6.19 [3.37; 10.12]</t>
+  </si>
+  <si>
+    <t>5.02 [2.23; 8.91]</t>
   </si>
 </sst>
 </file>
@@ -904,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -920,30 +920,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" s="12" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>153</v>
-      </c>
       <c r="E2" s="13" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -951,22 +951,22 @@
         <v>7</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>14</v>
+        <v>161</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>15</v>
+        <v>162</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>16</v>
+        <v>163</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>17</v>
+        <v>164</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>18</v>
+        <v>165</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>133</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -978,7 +978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
@@ -1004,46 +1004,46 @@
         <v>13</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>10</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="J1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="P1" s="9" t="s">
         <v>10</v>
@@ -1196,173 +1196,173 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B2" s="8">
         <v>0.73</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E2" s="8">
         <v>0.74</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B3" s="8">
         <v>0.71</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E3" s="8">
         <v>0.71</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B4" s="8">
         <v>0.57999999999999996</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E4" s="8">
         <v>0.62</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B7" s="8">
         <v>0.74</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E7" s="8">
         <v>0.71</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H7" s="8">
         <v>0.02</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="K7" s="8">
         <v>0.71</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="N7" s="8">
         <v>0.03</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B8" s="8">
         <v>0.69</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E8" s="8">
         <v>0.66</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="H8" s="8">
         <v>0.02</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K8" s="8">
         <v>0.66</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="N8" s="8">
         <v>0.03</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="B9" s="8">
         <v>0.68</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E9" s="8">
         <v>0.6</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="H9" s="8">
         <v>0.08</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K9" s="8">
         <v>0.62</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="N9" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -1571,10 +1571,10 @@
         <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="2"/>
@@ -1589,7 +1589,7 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F2" s="1">
         <v>41</v>
@@ -1600,19 +1600,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2">
         <v>1.25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D3" s="2">
         <v>0.98</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F3" s="1">
         <v>5</v>
@@ -1623,19 +1623,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2">
         <v>1.1100000000000001</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2">
         <v>1.29</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F4" s="1">
         <v>10</v>
@@ -1646,19 +1646,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2">
         <v>1.65</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D5" s="2">
         <v>1.4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F5" s="1">
         <v>28</v>
@@ -1669,7 +1669,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
@@ -1698,61 +1698,61 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2">
         <v>1.44</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D8" s="2">
         <v>1.08</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2">
         <v>1.5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D9" s="2">
         <v>1.1399999999999999</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2">
         <v>2.33</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D10" s="2">
         <v>1.53</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>0</v>
@@ -1781,73 +1781,73 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B13" s="2">
         <v>1.3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D13" s="2">
         <v>1.29</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2">
         <v>1.43</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D14" s="2">
         <v>1.39</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D15" s="2">
         <v>1.1499999999999999</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B16" s="2">
         <v>2.4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D16" s="2">
         <v>1.56</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F16" s="1">
         <v>147</v>
@@ -1858,19 +1858,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2">
         <v>1.52</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D17" s="2">
         <v>1.46</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F17" s="1">
         <v>11</v>
@@ -1881,19 +1881,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B18" s="2">
         <v>0.95</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D18" s="2">
         <v>0.95</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F18" s="1">
         <v>3</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1909,7 +1909,7 @@
         <v>0.98</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -1917,7 +1917,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1925,7 +1925,7 @@
         <v>3.61</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F20" s="1">
         <v>6</v>
@@ -1933,7 +1933,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1945,7 +1945,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1957,7 +1957,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1965,13 +1965,13 @@
         <v>1.4</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1979,13 +1979,13 @@
         <v>0.96</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1993,13 +1993,13 @@
         <v>0.9</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2007,7 +2007,7 @@
         <v>1.22</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F26" s="1"/>
     </row>
@@ -2019,7 +2019,7 @@
         <v>0.77</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -2033,7 +2033,7 @@
         <v>0.79</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -2222,10 +2222,10 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2238,7 +2238,7 @@
         <v>2.93</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F2" s="4">
         <v>138</v>
@@ -2246,19 +2246,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2">
         <v>1.21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D3" s="2">
         <v>1.21</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F3" s="4">
         <v>11</v>
@@ -2266,19 +2266,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
         <v>1.6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D4" s="2">
         <v>1.6</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F4" s="4">
         <v>32</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2297,7 +2297,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
@@ -2309,70 +2309,70 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2">
         <v>1.3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D7" s="2">
         <v>1.3</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2">
         <v>1.46</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D8" s="2">
         <v>1.46</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2">
         <v>1.98</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D9" s="2">
         <v>1.98</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2">
         <v>2.57</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D10" s="2">
         <v>1.59</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F10" s="4">
         <v>218</v>
@@ -2383,7 +2383,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2391,7 +2391,7 @@
         <v>5.15</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F11" s="4">
         <v>20</v>
@@ -2405,7 +2405,7 @@
         <v>0.76</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -2417,7 +2417,7 @@
         <v>0.79</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2"/>
     </row>
@@ -2477,10 +2477,10 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2493,7 +2493,7 @@
         <v>6.44</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F2" s="4">
         <v>38</v>
@@ -2504,19 +2504,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2">
         <v>1.65</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D3" s="2">
         <v>1.21</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F3" s="4">
         <v>12</v>
@@ -2527,19 +2527,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2">
         <v>0.93</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D4" s="2">
         <v>1.39</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F4" s="4">
         <v>8</v>
@@ -2550,19 +2550,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2">
         <v>2.06</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D5" s="2">
         <v>1.64</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F5" s="4">
         <v>30</v>
@@ -2573,7 +2573,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
@@ -2599,58 +2599,58 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2">
         <v>1.1299999999999999</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D8" s="2">
         <v>0.86</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2">
         <v>1.8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D9" s="2">
         <v>0.94</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2">
         <v>1.81</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D10" s="2">
         <v>1.56</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2664,7 +2664,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>0</v>
@@ -2676,70 +2676,70 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B13" s="2">
         <v>1.36</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D13" s="2">
         <v>1.1399999999999999</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2">
         <v>1.51</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D14" s="2">
         <v>1.27</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D15" s="2">
         <v>0.71</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B16" s="2">
         <v>2.54</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D16" s="2">
         <v>1.58</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F16" s="4">
         <v>76</v>
@@ -2750,19 +2750,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2">
         <v>1.22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D17" s="2">
         <v>1.49</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F17" s="4">
         <v>4</v>
@@ -2773,19 +2773,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B18" s="2">
         <v>0.94</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D18" s="2">
         <v>0.94</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F18" s="4">
         <v>2</v>
@@ -2793,7 +2793,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2801,7 +2801,7 @@
         <v>0.99</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -2809,7 +2809,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2817,7 +2817,7 @@
         <v>4.74</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F20" s="4">
         <v>4</v>
@@ -2825,7 +2825,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2836,7 +2836,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2846,7 +2846,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2854,12 +2854,12 @@
         <v>1.08</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2867,12 +2867,12 @@
         <v>1.23</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2880,12 +2880,12 @@
         <v>1.19</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2893,7 +2893,7 @@
         <v>1.42</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -2904,7 +2904,7 @@
         <v>0.8</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D27" s="2"/>
     </row>
@@ -3053,10 +3053,10 @@
         <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -3069,7 +3069,7 @@
         <v>3.4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F2" s="1">
         <v>87</v>
@@ -3078,19 +3078,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2">
         <v>1.18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D3" s="2">
         <v>1.18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F3" s="1">
         <v>4</v>
@@ -3099,19 +3099,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
         <v>1.83</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D4" s="2">
         <v>1.83</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F4" s="1">
         <v>30</v>
@@ -3120,7 +3120,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -3133,7 +3133,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
@@ -3147,71 +3147,71 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2">
         <v>0.96</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D7" s="2">
         <v>0.96</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2">
         <v>1.44</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D8" s="2">
         <v>1.44</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2">
         <v>1.74</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D9" s="2">
         <v>1.74</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2">
         <v>2.78</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D10" s="2">
         <v>1.6</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F10" s="1">
         <v>123</v>
@@ -3222,7 +3222,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3230,7 +3230,7 @@
         <v>7.27</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F11" s="1">
         <v>15</v>
@@ -3244,7 +3244,7 @@
         <v>0.79</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>

</xml_diff>

<commit_message>
Added analysis with pooled data
</commit_message>
<xml_diff>
--- a/Results/Results table.xlsx
+++ b/Results/Results table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14340" windowHeight="4215"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14340" windowHeight="4215" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="FU time" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="BS0.01" sheetId="2" r:id="rId5"/>
     <sheet name="Full model refit MSM" sheetId="3" r:id="rId6"/>
     <sheet name="BS0.01 refit MSM" sheetId="4" r:id="rId7"/>
+    <sheet name="Pooled data" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="181">
   <si>
     <t>(ref)</t>
   </si>
@@ -531,6 +532,48 @@
   </si>
   <si>
     <t>5.02 [2.23; 8.91]</t>
+  </si>
+  <si>
+    <t>[2.65; 3.34]</t>
+  </si>
+  <si>
+    <t>[1.45; 1.77]</t>
+  </si>
+  <si>
+    <t>[1.23; 1.71]</t>
+  </si>
+  <si>
+    <t>[1.10; 1.50]</t>
+  </si>
+  <si>
+    <t>[1.39; 1.98]</t>
+  </si>
+  <si>
+    <t>[1.05; 1.27]</t>
+  </si>
+  <si>
+    <t>Center</t>
+  </si>
+  <si>
+    <t>Covariates</t>
+  </si>
+  <si>
+    <t>Pooled data</t>
+  </si>
+  <si>
+    <t>Training data</t>
+  </si>
+  <si>
+    <t>[1.24; 1.42]</t>
+  </si>
+  <si>
+    <t>[1.90; 2.24]</t>
+  </si>
+  <si>
+    <t>[1.40; 1.77]</t>
+  </si>
+  <si>
+    <t>[3.28; 9.06]</t>
   </si>
 </sst>
 </file>
@@ -591,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -622,6 +665,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,7 +956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2197,7 +2249,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G13"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3020,7 +3072,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G12"/>
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3252,4 +3304,398 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="8" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.42578125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="G1" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2">
+        <v>2.93</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15">
+        <v>2.98</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15">
+        <v>1.33</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="I4" s="15">
+        <v>1.33</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15">
+        <v>1.6</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="I5" s="15">
+        <v>1.6</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15">
+        <v>1.45</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="I8" s="15">
+        <v>1.45</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.46</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.46</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15">
+        <v>1.28</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="I9" s="15">
+        <v>1.28</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15">
+        <v>1.66</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="I10" s="15">
+        <v>1.66</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2.57</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.59</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="I11" s="15">
+        <v>1.58</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15">
+        <v>5.45</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="I13" s="15">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="K13" s="6"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>